<commit_message>
update 1 delivery user stories
</commit_message>
<xml_diff>
--- a/DeliveryUserStory.xlsx
+++ b/DeliveryUserStory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbcdef5057a82b24/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbcdef5057a82b24/Documents/GitHub/Newsagent-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{40074C4C-EEE4-4437-A4A5-A7184A4C5235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FB6144C-444D-4281-8C9E-251B5ABA0569}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{40074C4C-EEE4-4437-A4A5-A7184A4C5235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E7776AB-7C2D-4EF9-B846-B8BD6753D775}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>User Story</t>
   </si>
@@ -56,34 +56,64 @@
     <t>As a Delivery Driver</t>
   </si>
   <si>
-    <t>I want to know what publications to put into my van</t>
-  </si>
-  <si>
-    <t>so the customer can get their subscription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I want to </t>
-  </si>
-  <si>
-    <t>so</t>
-  </si>
-  <si>
-    <t>I want to know how many of each publication I have to bring on my round</t>
-  </si>
-  <si>
-    <t>so I can give as many customers their subscription as I can</t>
-  </si>
-  <si>
-    <t>I want to know the date</t>
-  </si>
-  <si>
-    <t>so I can check it with today's date and know this is the right order</t>
-  </si>
-  <si>
-    <t>I want to see address and name of each customer beside each subscription</t>
-  </si>
-  <si>
-    <t>so I know who to deliver it to</t>
+    <t>Verify that 12 drivers have each logged in successfully</t>
+  </si>
+  <si>
+    <t>Verify that correct date is displayed</t>
+  </si>
+  <si>
+    <t>Verify that correct district is displayed</t>
+  </si>
+  <si>
+    <t>Verify that delivery docket can be printed successfully</t>
+  </si>
+  <si>
+    <t>Verify that errors are handled</t>
+  </si>
+  <si>
+    <t>I want to print delivery docket</t>
+  </si>
+  <si>
+    <t>so I can deliver the publications to the correct customer</t>
+  </si>
+  <si>
+    <t>I want to log into the system</t>
+  </si>
+  <si>
+    <t>so I can use the system</t>
+  </si>
+  <si>
+    <t>Verify that correct username is entered</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Verify that correct password is entered</t>
+  </si>
+  <si>
+    <t>username reflects district no.</t>
+  </si>
+  <si>
+    <t>Verify that publications summary is available</t>
+  </si>
+  <si>
+    <t>so I can get the publications from the warehouse</t>
+  </si>
+  <si>
+    <t>summary will include total number, name of each publication</t>
+  </si>
+  <si>
+    <t>Verify that delivery details are displayed</t>
+  </si>
+  <si>
+    <t>delivery details are name, address, publication, checkboxes</t>
+  </si>
+  <si>
+    <t>Verify that system logs out after print of delivery docket</t>
+  </si>
+  <si>
+    <t>I want to upload docket back to system</t>
   </si>
 </sst>
 </file>
@@ -128,19 +158,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -456,11 +501,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE66FCB5-4BF4-4903-BAAB-3414C50CE758}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,9 +514,10 @@
     <col min="2" max="2" width="63.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.1796875" customWidth="1"/>
+    <col min="5" max="5" width="52.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -480,8 +526,11 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -492,209 +541,116 @@
         <v>4</v>
       </c>
       <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
edited my user story
</commit_message>
<xml_diff>
--- a/DeliveryUserStory.xlsx
+++ b/DeliveryUserStory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbcdef5057a82b24/Documents/GitHub/Newsagent-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronan\OneDrive\Documents\GitHub\Newsagent-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{40074C4C-EEE4-4437-A4A5-A7184A4C5235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B09DC7E-475D-4145-B994-4915436CC5A0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14439FCE-C5CD-4B86-A903-60C3B147CFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4168C7-28B8-4B96-A04E-7170FD7B4563}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Acceptance Criteria</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                       </t>
+  </si>
+  <si>
+    <t>I want to print invoice</t>
   </si>
 </sst>
 </file>
@@ -199,10 +202,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,11 +501,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE66FCB5-4BF4-4903-BAAB-3414C50CE758}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,6 +649,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>

</xml_diff>